<commit_message>
Sd correction conceptmaps (#60)
* correction group target et source dans les CM

* correction warning name CM

[1, 2] ConceptMap: Warning - Rule cmd-0: 'Name should be usable as an identifier for the module by machine processing applications such as code generation' Failed

* Update ECLAIRELabel.fsh

suppr commentaires 9be367bbcf55221167c8ae9852832fee57ad4442
</commit_message>
<xml_diff>
--- a/ig/main/eclaire-study-phase-concept-map.xlsx
+++ b/ig/main/eclaire-study-phase-concept-map.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Mapping Table 0" r:id="rId4" sheetId="2"/>
+    <sheet name="Mapping Table 1" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>Property</t>
   </si>
@@ -36,7 +37,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>FHIR-Eclaire-phase-concept-map</t>
+    <t>FHIR_Eclaire_phase_concept_map</t>
   </si>
   <si>
     <t>Title</t>
@@ -60,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-04T08:22:22+00:00</t>
+    <t>2023-09-04T12:29:28+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -105,9 +106,15 @@
     <t>Relationship</t>
   </si>
   <si>
+    <t>eclaire-study-phase-source-code-system</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>http://terminology.hl7.org/CodeSystem/research-study-phase</t>
+  </si>
+  <si>
     <t>jarde-early</t>
   </si>
   <si>
@@ -159,10 +166,7 @@
     <t>phase-3</t>
   </si>
   <si>
-    <t>phase-IV</t>
-  </si>
-  <si>
-    <t>phase-4</t>
+    <t>eclaire-study-phase-code-system</t>
   </si>
   <si>
     <t>phase-III-IV</t>
@@ -435,7 +439,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -460,189 +464,223 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s" s="2">
         <v>36</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>34</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s" s="2">
         <v>36</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>34</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s" s="2">
         <v>36</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>34</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="2">
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s" s="2">
+      <c r="E2" t="s" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>